<commit_message>
Initial commit for Module 2 Activity
</commit_message>
<xml_diff>
--- a/tests/shape/test_plan_rectangle.xlsx
+++ b/tests/shape/test_plan_rectangle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rrcca-my.sharepoint.com/personal/skim14_rrc_ca/Documents/rrc_polytech/Fall_2024/intermediate_software_development/activities/activity_2/tests/shape/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a70c7754b2d0f532/Desktop/TERM2RRC/Intermideate Software Developer/Activities/activity_2/tests/shape/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{75D0B001-6057-4615-9964-5A71A3F0CEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A4FE063-91CF-49AC-92AF-7CFE36A16963}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{75D0B001-6057-4615-9964-5A71A3F0CEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{839261D3-5F8E-42C5-AF4A-7D39C5DC3706}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="28800" windowHeight="15370" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -248,9 +248,6 @@
     <t>Rectangle</t>
   </si>
   <si>
-    <t>Sion Kim</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -295,6 +292,9 @@
   </si>
   <si>
     <t>Perimeter: 18.00</t>
+  </si>
+  <si>
+    <t>Apurba Khan</t>
   </si>
 </sst>
 </file>
@@ -1155,22 +1155,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E9" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.73046875" customWidth="1"/>
-    <col min="3" max="3" width="22.265625" customWidth="1"/>
-    <col min="4" max="4" width="32.73046875" customWidth="1"/>
-    <col min="5" max="5" width="29.1328125" customWidth="1"/>
-    <col min="6" max="6" width="35.3984375" customWidth="1"/>
-    <col min="7" max="7" width="40.06640625" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="5" max="5" width="29.08984375" customWidth="1"/>
+    <col min="6" max="6" width="35.36328125" customWidth="1"/>
+    <col min="7" max="7" width="40.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="2.85">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="2.15">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1182,16 +1182,16 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1200,10 +1200,10 @@
       </c>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="11">
         <v>1</v>
@@ -1235,16 +1235,16 @@
         <v>11</v>
       </c>
       <c r="E7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="12">
         <v>2</v>
@@ -1256,16 +1256,16 @@
         <v>12</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="12">
         <v>3</v>
@@ -1277,16 +1277,16 @@
         <v>18</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="11">
         <v>4</v>
@@ -1298,16 +1298,16 @@
         <v>19</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="11">
         <v>5</v>
       </c>
@@ -1318,16 +1318,16 @@
         <v>14</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="12">
         <v>6</v>
       </c>
@@ -1338,16 +1338,16 @@
         <v>16</v>
       </c>
       <c r="E12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="12">
         <v>7</v>
       </c>
@@ -1358,16 +1358,16 @@
         <v>16</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="11">
         <v>8</v>
       </c>
@@ -1377,7 +1377,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="11">
         <v>9</v>
       </c>
@@ -1387,7 +1387,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="12">
         <v>10</v>
       </c>
@@ -1397,7 +1397,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="12">
         <v>11</v>
       </c>
@@ -1407,7 +1407,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="11">
         <v>12</v>
       </c>
@@ -1417,7 +1417,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="11">
         <v>13</v>
       </c>
@@ -1427,7 +1427,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="12">
         <v>14</v>
       </c>
@@ -1437,7 +1437,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="12">
         <v>15</v>
       </c>
@@ -1447,7 +1447,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>16</v>
       </c>
@@ -1457,7 +1457,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="11">
         <v>17</v>
       </c>
@@ -1467,7 +1467,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B25" s="19" t="s">
         <v>6</v>
       </c>

</xml_diff>